<commit_message>
23.08.2025 10:37  коррекция excel+buttons
</commit_message>
<xml_diff>
--- a/CRM_Project_Map.xlsx
+++ b/CRM_Project_Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\crm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{405B0995-ECD1-472E-A7BA-36CCCC5B4390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EDE453-A1AC-428E-98F8-844283ABC733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81B75E39-C69D-4058-94B9-F83317305778}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81B75E39-C69D-4058-94B9-F83317305778}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
   <si>
     <t>1.</t>
   </si>
@@ -93,13 +93,109 @@
   </si>
   <si>
     <t>столбцы</t>
+  </si>
+  <si>
+    <t>crm.db</t>
+  </si>
+  <si>
+    <t>app.py</t>
+  </si>
+  <si>
+    <t>гланый  модуль проекта, дипетчер функциональности</t>
+  </si>
+  <si>
+    <t>заголовки</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>загрузки from</t>
+  </si>
+  <si>
+    <t>load_dotenv()</t>
+  </si>
+  <si>
+    <t>ensure_schema()</t>
+  </si>
+  <si>
+    <t>модуль</t>
+  </si>
+  <si>
+    <t>Dispatcher()</t>
+  </si>
+  <si>
+    <r>
+      <t>Bot(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>token=TELEGRAM_TOKEN)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>_get_role_from_db</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(tg_id: int)</t>
+    </r>
+  </si>
+  <si>
+    <t>dp.include_router(arg)</t>
+  </si>
+  <si>
+    <t>аргументы, arg</t>
+  </si>
+  <si>
+    <t>start.router</t>
+  </si>
+  <si>
+    <t>registration.router</t>
+  </si>
+  <si>
+    <t>auth.router</t>
+  </si>
+  <si>
+    <t>info.router</t>
+  </si>
+  <si>
+    <t>schedule_router</t>
+  </si>
+  <si>
+    <r>
+      <t>cmd_start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFBCBEC4"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>(message: Message)</t>
+    </r>
+  </si>
+  <si>
+    <t>message.answer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +203,24 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBCBEC4"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF56A8F5"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,13 +243,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,302 +594,570 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700C8A7D-78BD-4FD3-B338-F6520A30FF8F}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:D32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="22.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1"/>
-    <col min="6" max="6" width="13.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.77734375" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="11.109375" style="5" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="5"/>
+    <col min="4" max="4" width="24.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.88671875" style="5" customWidth="1"/>
+    <col min="6" max="6" width="35.88671875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="5"/>
+    <col min="9" max="9" width="13.77734375" style="5" customWidth="1"/>
+    <col min="10" max="10" width="14.77734375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="12" style="5" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:13">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" ht="28.8">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" ht="68.400000000000006" customHeight="1">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="41.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" ht="50.4" customHeight="1">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="62.4" customHeight="1">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" ht="64.8" customHeight="1">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="41.4" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="E13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="G13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="J13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="K13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="L13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="M13" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="14" spans="1:13" ht="34.200000000000003" customHeight="1">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="2:12" ht="28.2">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="2:12" ht="34.200000000000003" customHeight="1">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="2:12">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="2:12">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="2:12">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="2:12">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="2:12">
+      <c r="B31" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="D31" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="I31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D29" s="2" t="s">
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="2:12">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="40" spans="2:12">
+      <c r="I40" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D30" s="2" t="s">
+    <row r="41" spans="2:12" ht="57.6">
+      <c r="I41" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D31" s="2" t="s">
+    <row r="42" spans="2:12" ht="57.6">
+      <c r="I42" s="4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>